<commit_message>
add test https errors
</commit_message>
<xml_diff>
--- a/Epochs/reports/report.xlsx
+++ b/Epochs/reports/report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1620,10 +1620,8 @@
           <t>object-detection</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>139863102765096</t>
-        </is>
+      <c r="C25" t="n">
+        <v>139863102765096</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -1650,11 +1648,7 @@
           <t>94%</t>
         </is>
       </c>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr">
         <is>
           <t>2025-04-29 16:35:46</t>
@@ -1675,10 +1669,8 @@
           <t>object-detection</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>139863102765096</t>
-        </is>
+      <c r="C26" t="n">
+        <v>139863102765096</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -1705,11 +1697,7 @@
           <t>95%</t>
         </is>
       </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr">
         <is>
           <t>2025-04-29 18:20:01</t>
@@ -1730,10 +1718,8 @@
           <t>object-detection</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>139863102765096</t>
-        </is>
+      <c r="C27" t="n">
+        <v>139863102765096</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -1760,11 +1746,7 @@
           <t>94%</t>
         </is>
       </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="I27" t="inlineStr"/>
       <c r="J27" t="inlineStr">
         <is>
           <t>2025-04-29 18:42:33</t>
@@ -1785,10 +1767,8 @@
           <t>classification</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>139863258720298</t>
-        </is>
+      <c r="C28" t="n">
+        <v>139863258720298</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -1815,11 +1795,7 @@
           <t>100%</t>
         </is>
       </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="I28" t="inlineStr"/>
       <c r="J28" t="inlineStr">
         <is>
           <t>2025-04-29 18:45:12</t>
@@ -1840,10 +1816,8 @@
           <t>classification</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>139863258720298</t>
-        </is>
+      <c r="C29" t="n">
+        <v>139863258720298</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -1870,11 +1844,7 @@
           <t>100%</t>
         </is>
       </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="I29" t="inlineStr"/>
       <c r="J29" t="inlineStr">
         <is>
           <t>2025-04-29 18:47:23</t>
@@ -1895,10 +1865,8 @@
           <t>classification</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>139863258720298</t>
-        </is>
+      <c r="C30" t="n">
+        <v>139863258720298</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -1925,11 +1893,7 @@
           <t>100%</t>
         </is>
       </c>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="I30" t="inlineStr"/>
       <c r="J30" t="inlineStr">
         <is>
           <t>2025-04-29 18:50:05</t>
@@ -1950,10 +1914,8 @@
           <t>segmentation</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>139863342313515</t>
-        </is>
+      <c r="C31" t="n">
+        <v>139863342313515</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -1980,11 +1942,7 @@
           <t>88%</t>
         </is>
       </c>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="I31" t="inlineStr"/>
       <c r="J31" t="inlineStr">
         <is>
           <t>2025-04-29 18:55:27</t>
@@ -2005,10 +1963,8 @@
           <t>segmentation</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>139863342313515</t>
-        </is>
+      <c r="C32" t="n">
+        <v>139863342313515</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -2035,11 +1991,7 @@
           <t>94%</t>
         </is>
       </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="I32" t="inlineStr"/>
       <c r="J32" t="inlineStr">
         <is>
           <t>2025-04-29 19:06:20</t>
@@ -2060,47 +2012,536 @@
           <t>segmentation</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
+      <c r="C33" t="n">
+        <v>139863342313515</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>11.97 minutes</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>SegFormer-[14M]</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>{'height': 800, 'width': 800, 'paddingValue': 0}</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>95%</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>92%</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr"/>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>2025-04-29 19:19:50</t>
+        </is>
+      </c>
+      <c r="K33" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Epochs</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>object-detection</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>139863102765096</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>7.02 minutes</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>RtmDet-[9M]</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>{'height': 600, 'width': 600, 'paddingValue': 0}</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>99%</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>93%</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>2025-06-10 11:20:27</t>
+        </is>
+      </c>
+      <c r="K34" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Epochs</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>object-detection</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>139863102765096</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>13.59 minutes</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>RepPoints-[20M]</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>{'height': 600, 'width': 600, 'paddingValue': 0}</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>95%</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>2025-06-10 11:36:13</t>
+        </is>
+      </c>
+      <c r="K35" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Epochs</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>object-detection</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>139863102765096</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>15.58 minutes</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>RepPoints-[37M]</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>{'height': 600, 'width': 600, 'paddingValue': 0}</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>96%</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>2025-06-10 11:54:32</t>
+        </is>
+      </c>
+      <c r="K36" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Epochs</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>classification</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>139863258720298</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>1.24 minutes</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>ConvNext-[29M]</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>{'height': 512, 'width': 512, 'paddingValue': 0}</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>2025-06-10 11:57:10</t>
+        </is>
+      </c>
+      <c r="K37" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Epochs</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>classification</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>139863258720298</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>0.73 minutes</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>ConvNext-[16M]</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>{'height': 512, 'width': 512, 'paddingValue': 0}</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>2025-06-10 12:00:02</t>
+        </is>
+      </c>
+      <c r="K38" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Epochs</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>classification</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>139863258720298</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>0.82 minutes</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>ConvNext-[16M]</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>{'height': 512, 'width': 512, 'paddingValue': 0}</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>2025-06-10 12:02:17</t>
+        </is>
+      </c>
+      <c r="K39" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Epochs</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>segmentation</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
         <is>
           <t>139863342313515</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>11.97 minutes</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>4.09 minutes</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
         <is>
           <t>SegFormer-[14M]</t>
         </is>
       </c>
-      <c r="F33" t="inlineStr">
+      <c r="F40" t="inlineStr">
         <is>
           <t>{'height': 800, 'width': 800, 'paddingValue': 0}</t>
         </is>
       </c>
-      <c r="G33" t="inlineStr">
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>94%</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>89%</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>2025-06-10 12:07:35</t>
+        </is>
+      </c>
+      <c r="K40" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Epochs</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>segmentation</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>139863342313515</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>9.59 minutes</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>FastVit-[14M]</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>{'height': 800, 'width': 800, 'paddingValue': 0}</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>96%</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>94%</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>2025-06-10 12:18:05</t>
+        </is>
+      </c>
+      <c r="K41" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Epochs</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>segmentation</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>139863342313515</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>12.06 minutes</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>SegFormer-[14M]</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>{'height': 800, 'width': 800, 'paddingValue': 0}</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
         <is>
           <t>95%</t>
         </is>
       </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>92%</t>
-        </is>
-      </c>
-      <c r="I33" t="inlineStr">
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>91%</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="J33" t="inlineStr">
-        <is>
-          <t>2025-04-29 19:19:50</t>
-        </is>
-      </c>
-      <c r="K33" t="n">
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>2025-06-10 12:31:35</t>
+        </is>
+      </c>
+      <c r="K42" t="n">
         <v>150</v>
       </c>
     </row>

</xml_diff>